<commit_message>
Enhance the link extraction from website,
</commit_message>
<xml_diff>
--- a/journal_list.xlsx
+++ b/journal_list.xlsx
@@ -3849,7 +3849,11 @@
           <t>http://www.euacademic.org/Default.aspx</t>
         </is>
       </c>
-      <c r="D171" t="inlineStr"/>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -3865,7 +3869,11 @@
           <t>http://www.eurchembull.com/index.php/ECB</t>
         </is>
       </c>
-      <c r="D172" t="inlineStr"/>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -3881,7 +3889,11 @@
           <t>http://www.eesej.eu/</t>
         </is>
       </c>
-      <c r="D173" t="inlineStr"/>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -3897,7 +3909,11 @@
           <t>http://www.eijsr.org/</t>
         </is>
       </c>
-      <c r="D174" t="inlineStr"/>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -3913,7 +3929,11 @@
           <t>http://www.cekinfo.org.uk/EIJST</t>
         </is>
       </c>
-      <c r="D175" t="inlineStr"/>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -3929,7 +3949,11 @@
           <t>http://euroessays.org/</t>
         </is>
       </c>
-      <c r="D176" t="inlineStr"/>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -3945,7 +3969,11 @@
           <t>http://eujcs.eu/</t>
         </is>
       </c>
-      <c r="D177" t="inlineStr"/>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -3961,7 +3989,11 @@
           <t>http://ejaet.com/theme.php?go=home</t>
         </is>
       </c>
-      <c r="D178" t="inlineStr"/>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -3977,7 +4009,11 @@
           <t>http://www.ejbps.com/</t>
         </is>
       </c>
-      <c r="D179" t="inlineStr"/>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -3993,7 +4029,11 @@
           <t>http://www.biotechjournal.info/</t>
         </is>
       </c>
-      <c r="D180" t="inlineStr"/>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -4009,7 +4049,11 @@
           <t>http://www.ejbss.com/home.aspx</t>
         </is>
       </c>
-      <c r="D181" t="inlineStr"/>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -4025,7 +4069,11 @@
           <t>http://www.eurjchem.com/index.php/eurjchem</t>
         </is>
       </c>
-      <c r="D182" t="inlineStr"/>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -4041,7 +4089,11 @@
           <t>http://ejcem.eu/</t>
         </is>
       </c>
-      <c r="D183" t="inlineStr"/>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -4057,7 +4109,11 @@
           <t>http://www.europeanjournalofeconomicsfinanceandadministrativesciences.com/</t>
         </is>
       </c>
-      <c r="D184" t="inlineStr"/>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -4073,7 +4129,11 @@
           <t>http://eurojedu.com/</t>
         </is>
       </c>
-      <c r="D185" t="inlineStr"/>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -4089,7 +4149,11 @@
           <t>http://www.ejes.eu/</t>
         </is>
       </c>
-      <c r="D186" t="inlineStr"/>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -4105,7 +4169,11 @@
           <t>http://www.ejers.org/index.php/ejers</t>
         </is>
       </c>
-      <c r="D187" t="inlineStr"/>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -4121,7 +4189,11 @@
           <t>http://world-science.ru/euro/</t>
         </is>
       </c>
-      <c r="D188" t="inlineStr"/>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -4137,7 +4209,11 @@
           <t>http://www.ejpmr.com/</t>
         </is>
       </c>
-      <c r="D189" t="inlineStr"/>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
@@ -4153,7 +4229,11 @@
           <t>http://www.ejst.tuiasi.ro/</t>
         </is>
       </c>
-      <c r="D190" t="inlineStr"/>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -4169,7 +4249,11 @@
           <t>http://www.europeanjournalofscientificresearch.com/</t>
         </is>
       </c>
-      <c r="D191" t="inlineStr"/>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -4185,7 +4269,11 @@
           <t>http://www.europeanjournalofsocialsciences.com/index.html</t>
         </is>
       </c>
-      <c r="D192" t="inlineStr"/>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -4201,7 +4289,11 @@
           <t>http://www.ecsdev.org/</t>
         </is>
       </c>
-      <c r="D193" t="inlineStr"/>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -4217,7 +4309,11 @@
           <t>http://elpjournal.eu/</t>
         </is>
       </c>
-      <c r="D194" t="inlineStr"/>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -4233,7 +4329,11 @@
           <t>http://european-science.com/eojnss/index</t>
         </is>
       </c>
-      <c r="D195" t="inlineStr"/>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
@@ -4249,7 +4349,11 @@
           <t>http://eujournal.org/index.php/esj</t>
         </is>
       </c>
-      <c r="D196" t="inlineStr"/>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -4265,7 +4369,11 @@
           <t>http://www.experimentjournal.com/</t>
         </is>
       </c>
-      <c r="D197" t="inlineStr"/>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -4281,7 +4389,11 @@
           <t>http://firjournal.com.ua/</t>
         </is>
       </c>
-      <c r="D198" t="inlineStr"/>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -4297,7 +4409,11 @@
           <t>http://www.fluidsjournal.org/</t>
         </is>
       </c>
-      <c r="D199" t="inlineStr"/>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -4313,7 +4429,11 @@
           <t>http://foodbiology.org/index.php/foodbio/</t>
         </is>
       </c>
-      <c r="D200" t="inlineStr"/>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
@@ -4329,7 +4449,11 @@
           <t>http://www.forexjournal.co.in/Index.aspx</t>
         </is>
       </c>
-      <c r="D201" t="inlineStr"/>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
@@ -4345,7 +4469,11 @@
           <t>http://www.fae-journal.org/index.aspx</t>
         </is>
       </c>
-      <c r="D202" t="inlineStr"/>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -4361,7 +4489,11 @@
           <t>http://jfatma.com/index.php</t>
         </is>
       </c>
-      <c r="D203" t="inlineStr"/>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
@@ -4377,7 +4509,11 @@
           <t>http://gjestenv.com/</t>
         </is>
       </c>
-      <c r="D204" t="inlineStr"/>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
@@ -4393,7 +4529,11 @@
           <t>http://www.galaxyimrj.com/</t>
         </is>
       </c>
-      <c r="D205" t="inlineStr"/>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -4409,7 +4549,11 @@
           <t>http://www.impactjournals.com/Genes&amp;Cancer/</t>
         </is>
       </c>
-      <c r="D206" t="inlineStr"/>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -4425,7 +4569,11 @@
           <t>http://gabi-journal.net/</t>
         </is>
       </c>
-      <c r="D207" t="inlineStr"/>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
@@ -4441,7 +4589,11 @@
           <t>http://www.geneticsmr.com/</t>
         </is>
       </c>
-      <c r="D208" t="inlineStr"/>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
@@ -4457,7 +4609,11 @@
           <t>http://www.geo-dynamica.com/</t>
         </is>
       </c>
-      <c r="D209" t="inlineStr"/>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -4473,7 +4629,11 @@
           <t>http://www.gbfrjournal.org/html/</t>
         </is>
       </c>
-      <c r="D210" t="inlineStr"/>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
@@ -4489,7 +4649,11 @@
           <t>http://worldwidejournals.com/gra/</t>
         </is>
       </c>
-      <c r="D211" t="inlineStr"/>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
@@ -4505,7 +4669,11 @@
           <t>http://www.gjaets.com/</t>
         </is>
       </c>
-      <c r="D212" t="inlineStr"/>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
@@ -4521,7 +4689,11 @@
           <t>http://www.gjar.org/</t>
         </is>
       </c>
-      <c r="D213" t="inlineStr"/>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -4537,7 +4709,11 @@
           <t>http://www.gjasr.com/</t>
         </is>
       </c>
-      <c r="D214" t="inlineStr"/>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
@@ -4553,7 +4729,11 @@
           <t>http://www.gjbss.com/</t>
         </is>
       </c>
-      <c r="D215" t="inlineStr"/>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
@@ -4569,7 +4749,11 @@
           <t>http://www.gjbssr.org/</t>
         </is>
       </c>
-      <c r="D216" t="inlineStr"/>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
@@ -4585,7 +4769,11 @@
           <t>http://www.gjesrm.com/</t>
         </is>
       </c>
-      <c r="D217" t="inlineStr"/>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
@@ -4601,7 +4789,11 @@
           <t>http://gjmst.com/index.htm</t>
         </is>
       </c>
-      <c r="D218" t="inlineStr"/>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -4617,7 +4809,11 @@
           <t>http://globaljmhs.org/</t>
         </is>
       </c>
-      <c r="D219" t="inlineStr"/>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -4633,7 +4829,11 @@
           <t>http://www.gjmedph.org/</t>
         </is>
       </c>
-      <c r="D220" t="inlineStr"/>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
@@ -4649,7 +4849,11 @@
           <t>http://www.gjms.co.in/index.php/gjms/index</t>
         </is>
       </c>
-      <c r="D221" t="inlineStr"/>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -4665,7 +4869,11 @@
           <t>http://www.globalmediajournal.com/</t>
         </is>
       </c>
-      <c r="D222" t="inlineStr"/>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -4681,7 +4889,11 @@
           <t>http://aygrt.isrj.org/Default.aspx</t>
         </is>
       </c>
-      <c r="D223" t="inlineStr"/>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -4697,7 +4909,11 @@
           <t>http://globalscholasticresearch.org/</t>
         </is>
       </c>
-      <c r="D224" t="inlineStr"/>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -4713,7 +4929,11 @@
           <t>http://ijtir.hctl.org/</t>
         </is>
       </c>
-      <c r="D225" t="inlineStr"/>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -4729,7 +4949,11 @@
           <t>http://revistahiperboreea.ro/</t>
         </is>
       </c>
-      <c r="D226" t="inlineStr"/>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -4745,7 +4969,11 @@
           <t>http://hortflorajournal.com/</t>
         </is>
       </c>
-      <c r="D227" t="inlineStr"/>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
@@ -4761,7 +4989,11 @@
           <t>http://www.hygeiajournal.com/</t>
         </is>
       </c>
-      <c r="D228" t="inlineStr"/>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -4777,7 +5009,11 @@
           <t>http://www.irj.iars.info/index.php</t>
         </is>
       </c>
-      <c r="D229" t="inlineStr"/>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
@@ -4793,7 +5029,11 @@
           <t>http://ijah.truescholar.org/</t>
         </is>
       </c>
-      <c r="D230" t="inlineStr"/>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
@@ -4809,7 +5049,11 @@
           <t>http://ijeas.truescholar.org/</t>
         </is>
       </c>
-      <c r="D231" t="inlineStr"/>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
@@ -4825,7 +5069,11 @@
           <t>http://ijems.truescholar.org/</t>
         </is>
       </c>
-      <c r="D232" t="inlineStr"/>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -4841,7 +5089,11 @@
           <t>http://ijopas.truescholar.org/</t>
         </is>
       </c>
-      <c r="D233" t="inlineStr"/>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -4857,7 +5109,11 @@
           <t>http://ijeps.truescholar.org/</t>
         </is>
       </c>
-      <c r="D234" t="inlineStr"/>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
@@ -4873,7 +5129,11 @@
           <t>http://ijopat.truescholar.org/</t>
         </is>
       </c>
-      <c r="D235" t="inlineStr"/>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
@@ -4889,7 +5149,11 @@
           <t>http://ijan.co.in/</t>
         </is>
       </c>
-      <c r="D236" t="inlineStr"/>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -4905,7 +5169,11 @@
           <t>http://www.ijacskros.com/index.html</t>
         </is>
       </c>
-      <c r="D237" t="inlineStr"/>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
@@ -4921,7 +5189,11 @@
           <t>http://www.themedicalacademy.in/</t>
         </is>
       </c>
-      <c r="D238" t="inlineStr"/>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -4937,7 +5209,11 @@
           <t>http://www.theglobaljournals.com/ijar/index.php</t>
         </is>
       </c>
-      <c r="D239" t="inlineStr"/>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -4953,7 +5229,11 @@
           <t>http://drugresearch.in/</t>
         </is>
       </c>
-      <c r="D240" t="inlineStr"/>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
@@ -4969,7 +5249,11 @@
           <t>http://www.ijmrps.com/</t>
         </is>
       </c>
-      <c r="D241" t="inlineStr"/>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -4985,7 +5269,11 @@
           <t>http://tnsroindia.org.in/journals.html</t>
         </is>
       </c>
-      <c r="D242" t="inlineStr"/>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -5001,7 +5289,11 @@
           <t>http://ijpbr.in/</t>
         </is>
       </c>
-      <c r="D243" t="inlineStr"/>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
@@ -5017,7 +5309,11 @@
           <t>http://www.ijpsrjournal.com/index.php</t>
         </is>
       </c>
-      <c r="D244" t="inlineStr"/>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -5033,7 +5329,11 @@
           <t>http://www.anvikshikijournal.com/</t>
         </is>
       </c>
-      <c r="D245" t="inlineStr"/>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
@@ -5049,7 +5349,11 @@
           <t>http://www.ijrpb.com/</t>
         </is>
       </c>
-      <c r="D246" t="inlineStr"/>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
@@ -5065,7 +5369,11 @@
           <t>http://www.ijsr.in/index.php</t>
         </is>
       </c>
-      <c r="D247" t="inlineStr"/>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -5081,7 +5389,11 @@
           <t>http://www.indjsrt.com/</t>
         </is>
       </c>
-      <c r="D248" t="inlineStr"/>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -5097,7 +5409,11 @@
           <t>http://irjps.in/</t>
         </is>
       </c>
-      <c r="D249" t="inlineStr"/>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
@@ -5113,7 +5429,11 @@
           <t>http://www.indianscholar.co.in/</t>
         </is>
       </c>
-      <c r="D250" t="inlineStr"/>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
@@ -5129,7 +5449,11 @@
           <t>http://isrj.org/Default.aspx</t>
         </is>
       </c>
-      <c r="D251" t="inlineStr"/>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -5145,7 +5469,11 @@
           <t>http://www.iajpr.com/</t>
         </is>
       </c>
-      <c r="D252" t="inlineStr"/>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
@@ -5161,7 +5489,11 @@
           <t>http://iajps.com/</t>
         </is>
       </c>
-      <c r="D253" t="inlineStr"/>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
@@ -5177,7 +5509,11 @@
           <t>http://iglobaljournal.com/</t>
         </is>
       </c>
-      <c r="D254" t="inlineStr"/>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
@@ -5193,7 +5529,11 @@
           <t>http://www.industrialscience.org/Default.aspx</t>
         </is>
       </c>
-      <c r="D255" t="inlineStr"/>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
@@ -5209,7 +5549,11 @@
           <t>http://www.information-iii.org/information_journal.html</t>
         </is>
       </c>
-      <c r="D256" t="inlineStr"/>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
@@ -5225,7 +5569,11 @@
           <t>http://www.innpharmacotherapy.com/Default.aspx</t>
         </is>
       </c>
-      <c r="D257" t="inlineStr"/>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
@@ -5241,7 +5589,11 @@
           <t>http://www.ieeeaj.com/</t>
         </is>
       </c>
-      <c r="D258" t="inlineStr"/>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
@@ -5257,7 +5609,11 @@
           <t>http://www.ijbritish.com/</t>
         </is>
       </c>
-      <c r="D259" t="inlineStr"/>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
@@ -5273,7 +5629,11 @@
           <t>http://ijcrb.webs.com/</t>
         </is>
       </c>
-      <c r="D260" t="inlineStr"/>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
@@ -5289,7 +5649,11 @@
           <t>http://www.idjrb.com/index.php</t>
         </is>
       </c>
-      <c r="D261" t="inlineStr"/>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
@@ -5305,7 +5669,11 @@
           <t>http://www.intertox.sav.sk/</t>
         </is>
       </c>
-      <c r="D262" t="inlineStr"/>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
@@ -5321,7 +5689,11 @@
           <t>http://internalmedicinereview.org/index.php/imr</t>
         </is>
       </c>
-      <c r="D263" t="inlineStr"/>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
@@ -5337,7 +5709,11 @@
           <t>http://iarjset.com/</t>
         </is>
       </c>
-      <c r="D264" t="inlineStr"/>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
@@ -5353,7 +5729,11 @@
           <t>http://iabcr.org/</t>
         </is>
       </c>
-      <c r="D265" t="inlineStr"/>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
@@ -5369,7 +5749,11 @@
           <t>http://www.intarchmed.com/</t>
         </is>
       </c>
-      <c r="D266" t="inlineStr"/>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
@@ -5385,7 +5769,11 @@
           <t>http://www.iamj.in/</t>
         </is>
       </c>
-      <c r="D267" t="inlineStr"/>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
@@ -5401,7 +5789,11 @@
           <t>http://www.tiarj.com/</t>
         </is>
       </c>
-      <c r="D268" t="inlineStr"/>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
@@ -5417,7 +5809,11 @@
           <t>http://journals.ke-i.org/index.php/IBR</t>
         </is>
       </c>
-      <c r="D269" t="inlineStr"/>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
@@ -5433,7 +5829,11 @@
           <t>http://www.internationalbulletinofbusinessadministration.com/</t>
         </is>
       </c>
-      <c r="D270" t="inlineStr"/>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
@@ -5449,7 +5849,11 @@
           <t>http://icfjournal.org/</t>
         </is>
       </c>
-      <c r="D271" t="inlineStr"/>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
@@ -5465,7 +5869,11 @@
           <t>http://journals.ke-i.org/index.php/icr</t>
         </is>
       </c>
-      <c r="D272" t="inlineStr"/>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
@@ -5481,7 +5889,11 @@
           <t>http://www.journal.faa-design.com/index.htm</t>
         </is>
       </c>
-      <c r="D273" t="inlineStr"/>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
@@ -5497,7 +5909,11 @@
           <t>http://www.ielonline.eu/</t>
         </is>
       </c>
-      <c r="D274" t="inlineStr"/>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
@@ -5513,7 +5929,11 @@
           <t>http://www.ierj.in/</t>
         </is>
       </c>
-      <c r="D275" t="inlineStr"/>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
@@ -5529,7 +5949,11 @@
           <t>http://oiirj.org/oiirj/ejournal/</t>
         </is>
       </c>
-      <c r="D276" t="inlineStr"/>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
@@ -5545,7 +5969,11 @@
           <t>http://iesrj.com/</t>
         </is>
       </c>
-      <c r="D277" t="inlineStr"/>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
@@ -5561,7 +5989,11 @@
           <t>http://iijoe.org/</t>
         </is>
       </c>
-      <c r="D278" t="inlineStr"/>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
@@ -5577,7 +6009,11 @@
           <t>http://www.iijsr.org/</t>
         </is>
       </c>
-      <c r="D279" t="inlineStr"/>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
@@ -5593,7 +6029,11 @@
           <t>http://www.ijmetmr.com/</t>
         </is>
       </c>
-      <c r="D280" t="inlineStr"/>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -5609,7 +6049,11 @@
           <t>http://www.ijassh.com/index.php</t>
         </is>
       </c>
-      <c r="D281" t="inlineStr"/>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -5625,7 +6069,11 @@
           <t>http://www.ijnmr.com/</t>
         </is>
       </c>
-      <c r="D282" t="inlineStr"/>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -5641,7 +6089,11 @@
           <t>http://www.ijarrp.com/</t>
         </is>
       </c>
-      <c r="D283" t="inlineStr"/>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -5657,7 +6109,11 @@
           <t>http://ijdcst.com/Default.aspx</t>
         </is>
       </c>
-      <c r="D284" t="inlineStr"/>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
@@ -5673,7 +6129,11 @@
           <t>http://www.ijier.net/</t>
         </is>
       </c>
-      <c r="D285" t="inlineStr"/>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
@@ -5689,7 +6149,11 @@
           <t>http://ijirmf.com/</t>
         </is>
       </c>
-      <c r="D286" t="inlineStr"/>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
@@ -5705,7 +6169,11 @@
           <t>http://www.ijirst.org/</t>
         </is>
       </c>
-      <c r="D287" t="inlineStr"/>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
@@ -5721,7 +6189,11 @@
           <t>http://www.ijmtst.com/index.html</t>
         </is>
       </c>
-      <c r="D288" t="inlineStr"/>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -5737,7 +6209,11 @@
           <t>http://www.ijprs.com/</t>
         </is>
       </c>
-      <c r="D289" t="inlineStr"/>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
@@ -5753,7 +6229,11 @@
           <t>http://ijrdt.org/</t>
         </is>
       </c>
-      <c r="D290" t="inlineStr"/>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
@@ -5769,7 +6249,11 @@
           <t>http://www.ijraset.com/</t>
         </is>
       </c>
-      <c r="D291" t="inlineStr"/>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
@@ -5785,7 +6269,11 @@
           <t>http://ijrest.net/</t>
         </is>
       </c>
-      <c r="D292" t="inlineStr"/>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
@@ -5801,7 +6289,11 @@
           <t>http://www.ijream.org/</t>
         </is>
       </c>
-      <c r="D293" t="inlineStr"/>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
@@ -5817,7 +6309,11 @@
           <t>http://www.ijsrd.com/</t>
         </is>
       </c>
-      <c r="D294" t="inlineStr"/>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
@@ -5833,7 +6329,11 @@
           <t>http://www.ijtre.com/home/</t>
         </is>
       </c>
-      <c r="D295" t="inlineStr"/>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
@@ -5849,7 +6349,11 @@
           <t>http://blackhorse.nazwa.pl/public_html/ojs/index.php/ijar</t>
         </is>
       </c>
-      <c r="D296" t="inlineStr"/>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
@@ -5865,7 +6369,11 @@
           <t>http://www.ijar.org.in/index.php</t>
         </is>
       </c>
-      <c r="D297" t="inlineStr"/>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
@@ -5881,7 +6389,11 @@
           <t>http://www.ijacademicstudies.com/</t>
         </is>
       </c>
-      <c r="D298" t="inlineStr"/>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
@@ -5897,7 +6409,11 @@
           <t>http://www.ijacta.com/index.php/ojs</t>
         </is>
       </c>
-      <c r="D299" t="inlineStr"/>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
@@ -5913,7 +6429,11 @@
           <t>http://www.ijaerd.com/</t>
         </is>
       </c>
-      <c r="D300" t="inlineStr"/>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
@@ -5929,7 +6449,11 @@
           <t>http://www.ijafrc.org/</t>
         </is>
       </c>
-      <c r="D301" t="inlineStr"/>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
@@ -5945,7 +6469,11 @@
           <t>http://ijafrse.org/</t>
         </is>
       </c>
-      <c r="D302" t="inlineStr"/>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
@@ -5961,7 +6489,11 @@
           <t>http://www.ijari.org/</t>
         </is>
       </c>
-      <c r="D303" t="inlineStr"/>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
@@ -5977,7 +6509,11 @@
           <t>http://ijariie.com/</t>
         </is>
       </c>
-      <c r="D304" t="inlineStr"/>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
@@ -5993,7 +6529,11 @@
           <t>http://www.ijariit.com/</t>
         </is>
       </c>
-      <c r="D305" t="inlineStr"/>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
@@ -6009,7 +6549,11 @@
           <t>http://www.ijarcsms.com/</t>
         </is>
       </c>
-      <c r="D306" t="inlineStr"/>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
@@ -6025,7 +6569,11 @@
           <t>http://www.ijarse.com/</t>
         </is>
       </c>
-      <c r="D307" t="inlineStr"/>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
@@ -6041,7 +6589,11 @@
           <t>http://www.ijaar.org/</t>
         </is>
       </c>
-      <c r="D308" t="inlineStr"/>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
@@ -6057,7 +6609,11 @@
           <t>http://www.science-gate.com/IJAAS.html</t>
         </is>
       </c>
-      <c r="D309" t="inlineStr"/>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
@@ -6073,7 +6629,11 @@
           <t>http://ijair.jctjournals.com/</t>
         </is>
       </c>
-      <c r="D310" t="inlineStr"/>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
@@ -6089,7 +6649,11 @@
           <t>http://www.ijact.org/</t>
         </is>
       </c>
-      <c r="D311" t="inlineStr"/>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
@@ -6105,7 +6669,11 @@
           <t>http://ijact.in/</t>
         </is>
       </c>
-      <c r="D312" t="inlineStr"/>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
@@ -6121,7 +6689,11 @@
           <t>http://www.alleducationjournal.com/</t>
         </is>
       </c>
-      <c r="D313" t="inlineStr"/>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
@@ -6137,7 +6709,11 @@
           <t>http://www.ijaemr.com/</t>
         </is>
       </c>
-      <c r="D314" t="inlineStr"/>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
@@ -6153,7 +6729,11 @@
           <t>http://www.ijaent.org/</t>
         </is>
       </c>
-      <c r="D315" t="inlineStr"/>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
@@ -6169,7 +6749,11 @@
           <t>http://fragrancejournals.com/</t>
         </is>
       </c>
-      <c r="D316" t="inlineStr"/>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
@@ -6185,7 +6769,11 @@
           <t>http://ijaems.com/</t>
         </is>
       </c>
-      <c r="D317" t="inlineStr"/>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
@@ -6201,7 +6789,11 @@
           <t>http://www.ijaera.org/</t>
         </is>
       </c>
-      <c r="D318" t="inlineStr"/>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
@@ -6217,7 +6809,11 @@
           <t>http://www.ijaers.com/</t>
         </is>
       </c>
-      <c r="D319" t="inlineStr"/>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
@@ -6233,7 +6829,11 @@
           <t>http://www.ader.org.in/</t>
         </is>
       </c>
-      <c r="D320" t="inlineStr"/>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
@@ -6249,7 +6849,11 @@
           <t>http://www.aestjournal.org/</t>
         </is>
       </c>
-      <c r="D321" t="inlineStr"/>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
@@ -6265,7 +6869,11 @@
           <t>http://www.ijaiasm.com/</t>
         </is>
       </c>
-      <c r="D322" t="inlineStr"/>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
@@ -6281,7 +6889,11 @@
           <t>http://www.ijaist.com/</t>
         </is>
       </c>
-      <c r="D323" t="inlineStr"/>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
@@ -6297,7 +6909,11 @@
           <t>http://ijals.com/</t>
         </is>
       </c>
-      <c r="D324" t="inlineStr"/>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
@@ -6313,7 +6929,11 @@
           <t>http://ijarm.com/index.html</t>
         </is>
       </c>
-      <c r="D325" t="inlineStr"/>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
@@ -6329,7 +6949,11 @@
           <t>http://www.ijana.in/</t>
         </is>
       </c>
-      <c r="D326" t="inlineStr"/>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
@@ -6345,7 +6969,11 @@
           <t>http://www.journalijar.com/index.php</t>
         </is>
       </c>
-      <c r="D327" t="inlineStr"/>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
@@ -6361,7 +6989,11 @@
           <t>http://www.ijarr.in/</t>
         </is>
       </c>
-      <c r="D328" t="inlineStr"/>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
@@ -6377,7 +7009,11 @@
           <t>http://ijarast.com/</t>
         </is>
       </c>
-      <c r="D329" t="inlineStr"/>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
@@ -6393,7 +7029,11 @@
           <t>http://www.ijarbs.com/</t>
         </is>
       </c>
-      <c r="D330" t="inlineStr"/>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
@@ -6409,7 +7049,11 @@
           <t>http://www.ijarbest.com/</t>
         </is>
       </c>
-      <c r="D331" t="inlineStr"/>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
@@ -6425,7 +7069,11 @@
           <t>http://www.ijarcce.com/</t>
         </is>
       </c>
-      <c r="D332" t="inlineStr"/>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
@@ -6441,7 +7089,11 @@
           <t>http://ijarcsee.org/index.php/IJARCSEE</t>
         </is>
       </c>
-      <c r="D333" t="inlineStr"/>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
@@ -6457,7 +7109,11 @@
           <t>http://www.ijarcsse.com/</t>
         </is>
       </c>
-      <c r="D334" t="inlineStr"/>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
@@ -6473,7 +7129,11 @@
           <t>http://www.ijarcst.com/index.html</t>
         </is>
       </c>
-      <c r="D335" t="inlineStr"/>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
@@ -6489,7 +7149,11 @@
           <t>http://ijaret.com/</t>
         </is>
       </c>
-      <c r="D336" t="inlineStr"/>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
@@ -6505,7 +7169,11 @@
           <t>http://www.ijareeie.com/</t>
         </is>
       </c>
-      <c r="D337" t="inlineStr"/>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
@@ -6521,7 +7189,11 @@
           <t>http://www.ijarem.org/</t>
         </is>
       </c>
-      <c r="D338" t="inlineStr"/>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
@@ -6537,7 +7209,11 @@
           <t>http://www.ijares.com/</t>
         </is>
       </c>
-      <c r="D339" t="inlineStr"/>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
@@ -6553,7 +7229,11 @@
           <t>http://ijarmet.com/</t>
         </is>
       </c>
-      <c r="D340" t="inlineStr"/>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
@@ -6569,7 +7249,11 @@
           <t>http://www.ijarst.com/</t>
         </is>
       </c>
-      <c r="D341" t="inlineStr"/>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
@@ -6585,7 +7269,11 @@
           <t>http://www.ijarset.com/</t>
         </is>
       </c>
-      <c r="D342" t="inlineStr"/>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
@@ -6601,7 +7289,11 @@
           <t>http://www.ijaset.com/</t>
         </is>
       </c>
-      <c r="D343" t="inlineStr"/>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
@@ -6617,7 +7309,11 @@
           <t>https://www.ijasrd.org/in/</t>
         </is>
       </c>
-      <c r="D344" t="inlineStr"/>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
@@ -6633,7 +7329,11 @@
           <t>http://www.ijatir.org/</t>
         </is>
       </c>
-      <c r="D345" t="inlineStr"/>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
@@ -6649,7 +7349,11 @@
           <t>http://www.ijates.com/</t>
         </is>
       </c>
-      <c r="D346" t="inlineStr"/>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
@@ -6665,7 +7369,11 @@
           <t>http://www.ijater.com/</t>
         </is>
       </c>
-      <c r="D347" t="inlineStr"/>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
@@ -6681,7 +7389,11 @@
           <t>http://www.ijats.org/</t>
         </is>
       </c>
-      <c r="D348" t="inlineStr"/>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
@@ -6697,7 +7409,11 @@
           <t>http://ijatca.com/</t>
         </is>
       </c>
-      <c r="D349" t="inlineStr"/>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
@@ -6713,7 +7429,11 @@
           <t>http://www.ijaetmas.com/</t>
         </is>
       </c>
-      <c r="D350" t="inlineStr"/>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
@@ -6729,7 +7449,11 @@
           <t>http://www.ijamae.uamae.org/editorial_board.html</t>
         </is>
       </c>
-      <c r="D351" t="inlineStr"/>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
@@ -6745,7 +7469,11 @@
           <t>http://www.ijoart.org/</t>
         </is>
       </c>
-      <c r="D352" t="inlineStr"/>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
@@ -6761,7 +7489,11 @@
           <t>http://www.ijaamm.com/</t>
         </is>
       </c>
-      <c r="D353" t="inlineStr"/>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
@@ -6777,7 +7509,11 @@
           <t>http://www.ijae.in/</t>
         </is>
       </c>
-      <c r="D354" t="inlineStr"/>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
@@ -6793,7 +7529,11 @@
           <t>http://www.ijaet.org/</t>
         </is>
       </c>
-      <c r="D355" t="inlineStr"/>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
@@ -6809,7 +7549,11 @@
           <t>http://international%20journal%20of%20advances%20in%20interdisciplinary%20research%20%28ijaidr%29/</t>
         </is>
       </c>
-      <c r="D356" t="inlineStr"/>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
@@ -6825,7 +7569,11 @@
           <t>http://www.managementjournal.info/</t>
         </is>
       </c>
-      <c r="D357" t="inlineStr"/>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
@@ -6841,7 +7589,11 @@
           <t>http://www.ijamee.info/</t>
         </is>
       </c>
-      <c r="D358" t="inlineStr"/>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
@@ -6857,7 +7609,11 @@
           <t>http://adv-math.com/</t>
         </is>
       </c>
-      <c r="D359" t="inlineStr"/>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
@@ -6873,7 +7629,11 @@
           <t>http://www.ijapronline.org/index.php</t>
         </is>
       </c>
-      <c r="D360" t="inlineStr"/>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
@@ -6889,7 +7649,11 @@
           <t>http://www.ijaps.org/Index/</t>
         </is>
       </c>
-      <c r="D361" t="inlineStr"/>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
@@ -6905,7 +7669,11 @@
           <t>http://ijarce.com/</t>
         </is>
       </c>
-      <c r="D362" t="inlineStr"/>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
@@ -6921,7 +7689,11 @@
           <t>http://www.ijamejournals.com/</t>
         </is>
       </c>
-      <c r="D363" t="inlineStr"/>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
@@ -6937,7 +7709,11 @@
           <t>http://ijagcs.com/</t>
         </is>
       </c>
-      <c r="D364" t="inlineStr"/>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
@@ -6953,7 +7729,11 @@
           <t>http://ijaer.in/index.php</t>
         </is>
       </c>
-      <c r="D365" t="inlineStr"/>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
@@ -6969,7 +7749,11 @@
           <t>http://ijair.org/</t>
         </is>
       </c>
-      <c r="D366" t="inlineStr"/>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
@@ -6985,7 +7769,11 @@
           <t>http://ijafp.com/</t>
         </is>
       </c>
-      <c r="D367" t="inlineStr"/>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
@@ -7001,7 +7789,11 @@
           <t>http://www.ijasvm.com/</t>
         </is>
       </c>
-      <c r="D368" t="inlineStr"/>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
@@ -7017,7 +7809,11 @@
           <t>http://www.ijappjournal.com/</t>
         </is>
       </c>
-      <c r="D369" t="inlineStr"/>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
@@ -7033,7 +7829,11 @@
           <t>http://www.ijaresm.com/</t>
         </is>
       </c>
-      <c r="D370" t="inlineStr"/>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
@@ -7049,7 +7849,11 @@
           <t>http://www.ijaiem.org/</t>
         </is>
       </c>
-      <c r="D371" t="inlineStr"/>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
@@ -7065,7 +7869,11 @@
           <t>http://ijapsa.com/</t>
         </is>
       </c>
-      <c r="D372" t="inlineStr"/>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
@@ -7081,7 +7889,11 @@
           <t>http://www.ijabpt.com/index.html</t>
         </is>
       </c>
-      <c r="D373" t="inlineStr"/>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
@@ -7097,7 +7909,11 @@
           <t>http://www.oraljournal.com/</t>
         </is>
       </c>
-      <c r="D374" t="inlineStr"/>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
@@ -7113,7 +7929,11 @@
           <t>http://sijournals.com/IJAE/</t>
         </is>
       </c>
-      <c r="D375" t="inlineStr"/>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
@@ -7129,7 +7949,11 @@
           <t>http://www.ijais.org/</t>
         </is>
       </c>
-      <c r="D376" t="inlineStr"/>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
@@ -7145,7 +7969,11 @@
           <t>http://www.journals.aiac.org.au/index.php/IJALEL</t>
         </is>
       </c>
-      <c r="D377" t="inlineStr"/>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
@@ -7161,7 +7989,11 @@
           <t>http://www.ijapbr.com/</t>
         </is>
       </c>
-      <c r="D378" t="inlineStr"/>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="n">
@@ -7177,7 +8009,11 @@
           <t>http://ijapsbs.com/</t>
         </is>
       </c>
-      <c r="D379" t="inlineStr"/>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
@@ -7193,7 +8029,11 @@
           <t>http://www.allresearchjournal.com/</t>
         </is>
       </c>
-      <c r="D380" t="inlineStr"/>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
@@ -7209,7 +8049,11 @@
           <t>http://www.ijars.in/</t>
         </is>
       </c>
-      <c r="D381" t="inlineStr"/>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
@@ -7225,7 +8069,11 @@
           <t>http://www.ijarnp.org/index.php/ijarnp</t>
         </is>
       </c>
-      <c r="D382" t="inlineStr"/>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
@@ -7241,7 +8089,11 @@
           <t>http://www.ijasem.com/</t>
         </is>
       </c>
-      <c r="D383" t="inlineStr"/>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
@@ -7257,7 +8109,11 @@
           <t>http://ijasbt.org/</t>
         </is>
       </c>
-      <c r="D384" t="inlineStr"/>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
@@ -7273,7 +8129,11 @@
           <t>http://www.ijapscengr.com/</t>
         </is>
       </c>
-      <c r="D385" t="inlineStr"/>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
@@ -7289,7 +8149,11 @@
           <t>http://iaajs.com/ijacu/</t>
         </is>
       </c>
-      <c r="D386" t="inlineStr"/>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
@@ -7305,7 +8169,11 @@
           <t>http://www.ijaim.org/</t>
         </is>
       </c>
-      <c r="D387" t="inlineStr"/>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
@@ -7321,7 +8189,11 @@
           <t>http://www.ijahs.com/</t>
         </is>
       </c>
-      <c r="D388" t="inlineStr"/>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
@@ -7337,7 +8209,11 @@
           <t>http://www.ijac.org.uk/</t>
         </is>
       </c>
-      <c r="D389" t="inlineStr"/>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
@@ -7353,7 +8229,11 @@
           <t>http://www.ijsse.org/index.php?option=com_content&amp;view=article&amp;id=67&amp;Itemid=63</t>
         </is>
       </c>
-      <c r="D390" t="inlineStr"/>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="n">

</xml_diff>

<commit_message>
fixed a bug in gethtml function
</commit_message>
<xml_diff>
--- a/journal_list.xlsx
+++ b/journal_list.xlsx
@@ -8249,7 +8249,11 @@
           <t>http://ijahms.com/</t>
         </is>
       </c>
-      <c r="D391" t="inlineStr"/>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
@@ -8265,7 +8269,11 @@
           <t>http://www.ijahss.com/</t>
         </is>
       </c>
-      <c r="D392" t="inlineStr"/>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
@@ -8281,7 +8289,11 @@
           <t>http://ijapr.in/</t>
         </is>
       </c>
-      <c r="D393" t="inlineStr"/>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
@@ -8297,7 +8309,11 @@
           <t>http://ijapc.com/</t>
         </is>
       </c>
-      <c r="D394" t="inlineStr"/>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
@@ -8313,7 +8329,11 @@
           <t>http://www.insikapub.com/</t>
         </is>
       </c>
-      <c r="D395" t="inlineStr"/>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
@@ -8329,7 +8349,11 @@
           <t>http://www.ijbmsp.org/index.php/IJBMSP/index</t>
         </is>
       </c>
-      <c r="D396" t="inlineStr"/>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
@@ -8345,7 +8369,11 @@
           <t>http://www.ijbsac.org/</t>
         </is>
       </c>
-      <c r="D397" t="inlineStr"/>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
@@ -8361,7 +8389,11 @@
           <t>https://scholarlyoa.com/individual-journals/International%20Journal%20of%20Basic%20Sciences%20and%20Applied%20Research%20(IJBSAR)</t>
         </is>
       </c>
-      <c r="D398" t="inlineStr"/>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
@@ -8377,7 +8409,11 @@
           <t>http://www.ijobio.com/</t>
         </is>
       </c>
-      <c r="D399" t="inlineStr"/>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
@@ -8393,7 +8429,11 @@
           <t>https://www.ijbio.com/index.php/ijb</t>
         </is>
       </c>
-      <c r="D400" t="inlineStr"/>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
@@ -8409,7 +8449,11 @@
           <t>http://www.ijbpr.com/</t>
         </is>
       </c>
-      <c r="D401" t="inlineStr"/>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
@@ -8425,7 +8469,11 @@
           <t>http://www.ifgdg.org/index.php?option=com_content&amp;view=featured&amp;Itemid=564</t>
         </is>
       </c>
-      <c r="D402" t="inlineStr"/>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="403">
       <c r="A403" t="n">
@@ -8441,7 +8489,11 @@
           <t>http://www.ijbpas.com/</t>
         </is>
       </c>
-      <c r="D403" t="inlineStr"/>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
@@ -8457,7 +8509,11 @@
           <t>http://www.ijbs.org/HomePage.aspx</t>
         </is>
       </c>
-      <c r="D404" t="inlineStr"/>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
@@ -8473,7 +8529,11 @@
           <t>http://ijbsans.com/index.html</t>
         </is>
       </c>
-      <c r="D405" t="inlineStr"/>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
@@ -8489,7 +8549,11 @@
           <t>http://www.ijbarr.com/</t>
         </is>
       </c>
-      <c r="D406" t="inlineStr"/>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="407">
       <c r="A407" t="n">
@@ -8505,7 +8569,11 @@
           <t>http://www.ijbcnet.com/</t>
         </is>
       </c>
-      <c r="D407" t="inlineStr"/>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="408">
       <c r="A408" t="n">
@@ -8521,7 +8589,11 @@
           <t>http://www.theijbm.com/</t>
         </is>
       </c>
-      <c r="D408" t="inlineStr"/>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="409">
       <c r="A409" t="n">
@@ -8537,7 +8609,11 @@
           <t>http://www.ijbmi.org/index.html</t>
         </is>
       </c>
-      <c r="D409" t="inlineStr"/>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="410">
       <c r="A410" t="n">
@@ -8553,7 +8629,11 @@
           <t>http://thejournalofbusiness.org/index.php/site</t>
         </is>
       </c>
-      <c r="D410" t="inlineStr"/>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="411">
       <c r="A411" t="n">
@@ -8569,7 +8649,11 @@
           <t>http://www.ijbmer.com/index.php</t>
         </is>
       </c>
-      <c r="D411" t="inlineStr"/>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="412">
       <c r="A412" t="n">
@@ -8585,7 +8669,11 @@
           <t>http://www.ijbmes.com/</t>
         </is>
       </c>
-      <c r="D412" t="inlineStr"/>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="413">
       <c r="A413" t="n">
@@ -8601,7 +8689,11 @@
           <t>http://www.ijbmm.com/</t>
         </is>
       </c>
-      <c r="D413" t="inlineStr"/>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="414">
       <c r="A414" t="n">
@@ -8617,7 +8709,11 @@
           <t>http://ijbemr.com/</t>
         </is>
       </c>
-      <c r="D414" t="inlineStr"/>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="415">
       <c r="A415" t="n">
@@ -8633,7 +8729,11 @@
           <t>http://www.ijbts-journal.com/</t>
         </is>
       </c>
-      <c r="D415" t="inlineStr"/>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="416">
       <c r="A416" t="n">
@@ -8649,7 +8749,11 @@
           <t>http://www.casestudiesjournal.com/</t>
         </is>
       </c>
-      <c r="D416" t="inlineStr"/>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="417">
       <c r="A417" t="n">
@@ -8665,7 +8769,11 @@
           <t>http://www.ijcps.com/</t>
         </is>
       </c>
-      <c r="D417" t="inlineStr"/>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="418">
       <c r="A418" t="n">
@@ -8681,7 +8789,11 @@
           <t>http://www.ijcst.net/</t>
         </is>
       </c>
-      <c r="D418" t="inlineStr"/>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="419">
       <c r="A419" t="n">
@@ -8697,7 +8809,11 @@
           <t>http://www.chemijournal.com/</t>
         </is>
       </c>
-      <c r="D419" t="inlineStr"/>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="420">
       <c r="A420" t="n">
@@ -8713,7 +8829,11 @@
           <t>http://ijcmes.com/</t>
         </is>
       </c>
-      <c r="D420" t="inlineStr"/>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="421">
       <c r="A421" t="n">
@@ -8729,7 +8849,11 @@
           <t>http://ijcdr.net/index.php</t>
         </is>
       </c>
-      <c r="D421" t="inlineStr"/>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="422">
       <c r="A422" t="n">
@@ -8745,7 +8869,11 @@
           <t>http://ijcci.info/</t>
         </is>
       </c>
-      <c r="D422" t="inlineStr"/>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="423">
       <c r="A423" t="n">
@@ -8761,7 +8889,11 @@
           <t>http://www.iomcworld.com/ijcrimph/</t>
         </is>
       </c>
-      <c r="D423" t="inlineStr"/>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="424">
       <c r="A424" t="n">
@@ -8777,7 +8909,11 @@
           <t>http://www.managejournal.com/</t>
         </is>
       </c>
-      <c r="D424" t="inlineStr"/>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="425">
       <c r="A425" t="n">
@@ -8793,7 +8929,11 @@
           <t>http://communicationandhealth.ro/</t>
         </is>
       </c>
-      <c r="D425" t="inlineStr"/>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="426">
       <c r="A426" t="n">
@@ -8809,7 +8949,11 @@
           <t>http://www.ijcnis.org/</t>
         </is>
       </c>
-      <c r="D426" t="inlineStr"/>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="427">
       <c r="A427" t="n">
@@ -8825,7 +8969,11 @@
           <t>http://ijcrbs.com/index.php</t>
         </is>
       </c>
-      <c r="D427" t="inlineStr"/>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="428">
       <c r="A428" t="n">
@@ -8841,7 +8989,11 @@
           <t>https://ijocaas.com/</t>
         </is>
       </c>
-      <c r="D428" t="inlineStr"/>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="429">
       <c r="A429" t="n">
@@ -8857,7 +9009,11 @@
           <t>http://www.ijceronline.com/</t>
         </is>
       </c>
-      <c r="D429" t="inlineStr"/>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="430">
       <c r="A430" t="n">
@@ -8873,7 +9029,11 @@
           <t>http://www.ijcsme.com/</t>
         </is>
       </c>
-      <c r="D430" t="inlineStr"/>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="431">
       <c r="A431" t="n">
@@ -8889,7 +9049,11 @@
           <t>http://ijcer.org/</t>
         </is>
       </c>
-      <c r="D431" t="inlineStr"/>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="432">
       <c r="A432" t="n">
@@ -8905,7 +9069,11 @@
           <t>http://www.ijccer.org/</t>
         </is>
       </c>
-      <c r="D432" t="inlineStr"/>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="433">
       <c r="A433" t="n">
@@ -8921,7 +9089,11 @@
           <t>http://www.ijcit.com/</t>
         </is>
       </c>
-      <c r="D433" t="inlineStr"/>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="434">
       <c r="A434" t="n">
@@ -8937,7 +9109,11 @@
           <t>http://www.ijcaonline.org/</t>
         </is>
       </c>
-      <c r="D434" t="inlineStr"/>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="435">
       <c r="A435" t="n">
@@ -8953,7 +9129,11 @@
           <t>http://www.ijcaet.net/</t>
         </is>
       </c>
-      <c r="D435" t="inlineStr"/>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="436">
       <c r="A436" t="n">
@@ -8969,7 +9149,11 @@
           <t>http://www.caesjournals.org/</t>
         </is>
       </c>
-      <c r="D436" t="inlineStr"/>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="437">
       <c r="A437" t="n">
@@ -8985,7 +9169,11 @@
           <t>http://www.ijcat.com/Default</t>
         </is>
       </c>
-      <c r="D437" t="inlineStr"/>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="438">
       <c r="A438" t="n">
@@ -9001,7 +9189,11 @@
           <t>http://www.ijcea.com/</t>
         </is>
       </c>
-      <c r="D438" t="inlineStr"/>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="439">
       <c r="A439" t="n">
@@ -9017,7 +9209,11 @@
           <t>http://ijcert.org/</t>
         </is>
       </c>
-      <c r="D439" t="inlineStr"/>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="440">
       <c r="A440" t="n">
@@ -9033,7 +9229,11 @@
           <t>http://www.ijcna.org/</t>
         </is>
       </c>
-      <c r="D440" t="inlineStr"/>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="441">
       <c r="A441" t="n">
@@ -9049,7 +9249,11 @@
           <t>http://ijcncs.org/</t>
         </is>
       </c>
-      <c r="D441" t="inlineStr"/>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="442">
       <c r="A442" t="n">
@@ -9065,7 +9269,11 @@
           <t>http://www.ijcscs.org/</t>
         </is>
       </c>
-      <c r="D442" t="inlineStr"/>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="443">
       <c r="A443" t="n">
@@ -9081,7 +9289,11 @@
           <t>http://www.ijcsbi.org/index.php/ijcsbi</t>
         </is>
       </c>
-      <c r="D443" t="inlineStr"/>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="444">
       <c r="A444" t="n">
@@ -9097,7 +9309,11 @@
           <t>http://www.ijcscn.com/</t>
         </is>
       </c>
-      <c r="D444" t="inlineStr"/>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="445">
       <c r="A445" t="n">
@@ -9113,7 +9329,11 @@
           <t>https://sites.google.com/site/ijcsis/</t>
         </is>
       </c>
-      <c r="D445" t="inlineStr"/>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="446">
       <c r="A446" t="n">
@@ -9129,7 +9349,11 @@
           <t>http://www.ijcsit.com/index.php</t>
         </is>
       </c>
-      <c r="D446" t="inlineStr"/>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="447">
       <c r="A447" t="n">
@@ -9145,7 +9369,11 @@
           <t>http://www.ijcsmc.com/</t>
         </is>
       </c>
-      <c r="D447" t="inlineStr"/>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="448">
       <c r="A448" t="n">
@@ -9161,7 +9389,11 @@
           <t>http://ijcsn.org/</t>
         </is>
       </c>
-      <c r="D448" t="inlineStr"/>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="449">
       <c r="A449" t="n">
@@ -9177,7 +9409,11 @@
           <t>http://ijcsns.org/</t>
         </is>
       </c>
-      <c r="D449" t="inlineStr"/>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="450">
       <c r="A450" t="n">
@@ -9193,7 +9429,11 @@
           <t>http://ijcsse.org/</t>
         </is>
       </c>
-      <c r="D450" t="inlineStr"/>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="451">
       <c r="A451" t="n">
@@ -9209,7 +9449,11 @@
           <t>http://ijcst.com/</t>
         </is>
       </c>
-      <c r="D451" t="inlineStr"/>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="452">
       <c r="A452" t="n">
@@ -9225,7 +9469,11 @@
           <t>http://www.ijcst.org/</t>
         </is>
       </c>
-      <c r="D452" t="inlineStr"/>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="453">
       <c r="A453" t="n">
@@ -9241,7 +9489,11 @@
           <t>http://www.ijcse.net/index.php</t>
         </is>
       </c>
-      <c r="D453" t="inlineStr"/>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="454">
       <c r="A454" t="n">
@@ -9257,7 +9509,11 @@
           <t>http://ijcset.net/</t>
         </is>
       </c>
-      <c r="D454" t="inlineStr"/>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="455">
       <c r="A455" t="n">
@@ -9273,7 +9529,11 @@
           <t>http://ijcsits.org/</t>
         </is>
       </c>
-      <c r="D455" t="inlineStr"/>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="456">
       <c r="A456" t="n">
@@ -9289,7 +9549,11 @@
           <t>http://ijcsi.org/index.php</t>
         </is>
       </c>
-      <c r="D456" t="inlineStr"/>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="457">
       <c r="A457" t="n">
@@ -9305,7 +9569,11 @@
           <t>http://www.ijcstjournal.org/</t>
         </is>
       </c>
-      <c r="D457" t="inlineStr"/>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="458">
       <c r="A458" t="n">
@@ -9321,7 +9589,11 @@
           <t>http://www.ijcsonline.com/</t>
         </is>
       </c>
-      <c r="D458" t="inlineStr"/>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="459">
       <c r="A459" t="n">
@@ -9337,7 +9609,11 @@
           <t>http://www.ijcta.com/index.php</t>
         </is>
       </c>
-      <c r="D459" t="inlineStr"/>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="460">
       <c r="A460" t="n">
@@ -9353,7 +9629,11 @@
           <t>http://www.ijctee.org/</t>
         </is>
       </c>
-      <c r="D460" t="inlineStr"/>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="461">
       <c r="A461" t="n">
@@ -9369,7 +9649,11 @@
           <t>http://www.meacse.org/ijcar/</t>
         </is>
       </c>
-      <c r="D461" t="inlineStr"/>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="462">
       <c r="A462" t="n">
@@ -9385,7 +9669,11 @@
           <t>http://www.ijccr.com/</t>
         </is>
       </c>
-      <c r="D462" t="inlineStr"/>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="463">
       <c r="A463" t="n">
@@ -9401,7 +9689,11 @@
           <t>http://ijcsit.org/</t>
         </is>
       </c>
-      <c r="D463" t="inlineStr"/>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="464">
       <c r="A464" t="n">
@@ -9417,7 +9709,11 @@
           <t>http://jocponline.com/</t>
         </is>
       </c>
-      <c r="D464" t="inlineStr"/>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="465">
       <c r="A465" t="n">
@@ -9433,7 +9729,11 @@
           <t>http://ijcas.net/</t>
         </is>
       </c>
-      <c r="D465" t="inlineStr"/>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="466">
       <c r="A466" t="n">
@@ -9449,7 +9749,11 @@
           <t>http://www.ijcmr.com/</t>
         </is>
       </c>
-      <c r="D466" t="inlineStr"/>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="467">
       <c r="A467" t="n">
@@ -9465,7 +9769,11 @@
           <t>http://ijcrr.in/index.php/ijcrr</t>
         </is>
       </c>
-      <c r="D467" t="inlineStr"/>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="468">
       <c r="A468" t="n">
@@ -9481,7 +9789,11 @@
           <t>http://ijcem.in/</t>
         </is>
       </c>
-      <c r="D468" t="inlineStr"/>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="469">
       <c r="A469" t="n">
@@ -9497,7 +9809,11 @@
           <t>http://journalijcar.org/</t>
         </is>
       </c>
-      <c r="D469" t="inlineStr"/>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="470">
       <c r="A470" t="n">
@@ -9513,7 +9829,11 @@
           <t>http://www.journalijcas.com/</t>
         </is>
       </c>
-      <c r="D470" t="inlineStr"/>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="471">
       <c r="A471" t="n">
@@ -9529,7 +9849,11 @@
           <t>https://scholarlyoa.com/individual-journals/International%20Journal%20of%20Current%20Business%20and%20Social%20Sciences%20(IJCBSS)</t>
         </is>
       </c>
-      <c r="D471" t="inlineStr"/>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="472">
       <c r="A472" t="n">
@@ -9545,7 +9869,11 @@
           <t>http://www.journalijces.com/</t>
         </is>
       </c>
-      <c r="D472" t="inlineStr"/>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="473">
       <c r="A473" t="n">
@@ -9561,7 +9889,11 @@
           <t>http://journalijcir.com/</t>
         </is>
       </c>
-      <c r="D473" t="inlineStr"/>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="474">
       <c r="A474" t="n">
@@ -9577,7 +9909,11 @@
           <t>http://journalcmpr.com/</t>
         </is>
       </c>
-      <c r="D474" t="inlineStr"/>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="475">
       <c r="A475" t="n">
@@ -9593,7 +9929,11 @@
           <t>http://journalijcmes.com/</t>
         </is>
       </c>
-      <c r="D475" t="inlineStr"/>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="476">
       <c r="A476" t="n">
@@ -9609,7 +9949,11 @@
           <t>http://www.ijcmas.com/</t>
         </is>
       </c>
-      <c r="D476" t="inlineStr"/>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="477">
       <c r="A477" t="n">
@@ -9625,7 +9969,11 @@
           <t>http://international%20journal%20of%20current%20multidisciplinary%20studies/</t>
         </is>
       </c>
-      <c r="D477" t="inlineStr"/>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="478">
       <c r="A478" t="n">
@@ -9641,7 +9989,11 @@
           <t>http://ijcpr.com/</t>
         </is>
       </c>
-      <c r="D478" t="inlineStr"/>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="479">
       <c r="A479" t="n">
@@ -9657,7 +10009,11 @@
           <t>http://www.journalcra.com/</t>
         </is>
       </c>
-      <c r="D479" t="inlineStr"/>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="480">
       <c r="A480" t="n">
@@ -9673,7 +10029,11 @@
           <t>http://www.ijcrar.com/</t>
         </is>
       </c>
-      <c r="D480" t="inlineStr"/>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="481">
       <c r="A481" t="n">
@@ -9689,7 +10049,11 @@
           <t>http://www.ijcrr.com/current_issue.html</t>
         </is>
       </c>
-      <c r="D481" t="inlineStr"/>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="482">
       <c r="A482" t="n">
@@ -9705,7 +10069,11 @@
           <t>http://www.ijcrcps.com/</t>
         </is>
       </c>
-      <c r="D482" t="inlineStr"/>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="483">
       <c r="A483" t="n">
@@ -9721,7 +10089,11 @@
           <t>http://www.ijcrls.com/</t>
         </is>
       </c>
-      <c r="D483" t="inlineStr"/>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="484">
       <c r="A484" t="n">
@@ -9737,7 +10109,11 @@
           <t>http://www.ijcrm.com/</t>
         </is>
       </c>
-      <c r="D484" t="inlineStr"/>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="485">
       <c r="A485" t="n">
@@ -9753,7 +10129,11 @@
           <t>http://currentsciencejournal.info/index.html</t>
         </is>
       </c>
-      <c r="D485" t="inlineStr"/>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="486">
       <c r="A486" t="n">
@@ -9769,7 +10149,11 @@
           <t>http://www.journalijcst.com/</t>
         </is>
       </c>
-      <c r="D486" t="inlineStr"/>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="487">
       <c r="A487" t="n">
@@ -9785,7 +10169,11 @@
           <t>http://www.ijdhs.com/home.html</t>
         </is>
       </c>
-      <c r="D487" t="inlineStr"/>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="488">
       <c r="A488" t="n">
@@ -9801,7 +10189,11 @@
           <t>http://dermatopathologyjournal.com/</t>
         </is>
       </c>
-      <c r="D488" t="inlineStr"/>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="489">
       <c r="A489" t="n">
@@ -9817,7 +10209,11 @@
           <t>http://isdsnet.com/journal.html</t>
         </is>
       </c>
-      <c r="D489" t="inlineStr"/>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="490">
       <c r="A490" t="n">
@@ -9833,7 +10229,11 @@
           <t>http://www.journalijdr.com/</t>
         </is>
       </c>
-      <c r="D490" t="inlineStr"/>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="491">
       <c r="A491" t="n">
@@ -9849,7 +10249,11 @@
           <t>http://ijdcn.co.in/</t>
         </is>
       </c>
-      <c r="D491" t="inlineStr"/>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="492">
       <c r="A492" t="n">
@@ -9865,7 +10269,11 @@
           <t>http://www.ijodls.in/</t>
         </is>
       </c>
-      <c r="D492" t="inlineStr"/>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="493">
       <c r="A493" t="n">
@@ -9881,7 +10289,11 @@
           <t>http://www.ijddr.in/</t>
         </is>
       </c>
-      <c r="D493" t="inlineStr"/>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="494">
       <c r="A494" t="n">
@@ -9897,7 +10309,11 @@
           <t>http://www.ijecse.com/</t>
         </is>
       </c>
-      <c r="D494" t="inlineStr"/>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="495">
       <c r="A495" t="n">
@@ -9913,7 +10329,11 @@
           <t>http://www.ijsse.org/index.php?option=com_content&amp;view=article&amp;id=548&amp;Itemid=82</t>
         </is>
       </c>
-      <c r="D495" t="inlineStr"/>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="496">
       <c r="A496" t="n">
@@ -9929,7 +10349,11 @@
           <t>http://www.ijeronline.com/</t>
         </is>
       </c>
-      <c r="D496" t="inlineStr"/>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="497">
       <c r="A497" t="n">
@@ -9945,7 +10369,11 @@
           <t>http://ijecm.co.uk/</t>
         </is>
       </c>
-      <c r="D497" t="inlineStr"/>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="498">
       <c r="A498" t="n">
@@ -9961,7 +10389,11 @@
           <t>http://www.ejournalofbusiness.org/</t>
         </is>
       </c>
-      <c r="D498" t="inlineStr"/>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="499">
       <c r="A499" t="n">
@@ -9977,7 +10409,11 @@
           <t>http://ijear.org/</t>
         </is>
       </c>
-      <c r="D499" t="inlineStr"/>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="500">
       <c r="A500" t="n">
@@ -9993,7 +10429,11 @@
           <t>http://ijepr.org/</t>
         </is>
       </c>
-      <c r="D500" t="inlineStr"/>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="501">
       <c r="A501" t="n">
@@ -10009,7 +10449,11 @@
           <t>http://www.ijern.com/index.php</t>
         </is>
       </c>
-      <c r="D501" t="inlineStr"/>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="502">
       <c r="A502" t="n">
@@ -10025,7 +10469,11 @@
           <t>http://www.ijessnet.com/</t>
         </is>
       </c>
-      <c r="D502" t="inlineStr"/>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="503">
       <c r="A503" t="n">
@@ -10041,7 +10489,11 @@
           <t>https://sites.google.com/site/tijepa2012/home</t>
         </is>
       </c>
-      <c r="D503" t="inlineStr"/>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="504">
       <c r="A504" t="n">
@@ -10057,7 +10509,11 @@
           <t>http://www.ijeionline.com/</t>
         </is>
       </c>
-      <c r="D504" t="inlineStr"/>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="505">
       <c r="A505" t="n">
@@ -10073,7 +10529,11 @@
           <t>http://www.arresearchpublication.com/</t>
         </is>
       </c>
-      <c r="D505" t="inlineStr"/>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="506">
       <c r="A506" t="n">
@@ -10089,7 +10549,11 @@
           <t>http://eecjournal.com/</t>
         </is>
       </c>
-      <c r="D506" t="inlineStr"/>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="507">
       <c r="A507" t="n">
@@ -10105,7 +10569,11 @@
           <t>http://www.ijeemc.com/</t>
         </is>
       </c>
-      <c r="D507" t="inlineStr"/>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="508">
       <c r="A508" t="n">
@@ -10121,7 +10589,11 @@
           <t>http://www.ijoee.org/</t>
         </is>
       </c>
-      <c r="D508" t="inlineStr"/>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="509">
       <c r="A509" t="n">
@@ -10137,7 +10609,11 @@
           <t>http://www.electrochemsci.org/</t>
         </is>
       </c>
-      <c r="D509" t="inlineStr"/>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="510">
       <c r="A510" t="n">
@@ -10153,7 +10629,11 @@
           <t>http://iject.org/</t>
         </is>
       </c>
-      <c r="D510" t="inlineStr"/>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="511">
       <c r="A511" t="n">
@@ -10169,7 +10649,11 @@
           <t>http://ijeie.jalaxy.com.tw/</t>
         </is>
       </c>
-      <c r="D511" t="inlineStr"/>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="512">
       <c r="A512" t="n">
@@ -10185,7 +10669,11 @@
           <t>http://www.ijecce.org/</t>
         </is>
       </c>
-      <c r="D512" t="inlineStr"/>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="513">
       <c r="A513" t="n">
@@ -10201,7 +10689,11 @@
           <t>http://www.ijecct.org/index.htm</t>
         </is>
       </c>
-      <c r="D513" t="inlineStr"/>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="514">
       <c r="A514" t="n">
@@ -10217,7 +10709,11 @@
           <t>http://www.ijeert.org/</t>
         </is>
       </c>
-      <c r="D514" t="inlineStr"/>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="515">
       <c r="A515" t="n">
@@ -10233,7 +10729,11 @@
           <t>http://www.ermt.net/</t>
         </is>
       </c>
-      <c r="D515" t="inlineStr"/>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="516">
       <c r="A516" t="n">
@@ -10249,7 +10749,11 @@
           <t>http://www.ijese.org/</t>
         </is>
       </c>
-      <c r="D516" t="inlineStr"/>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="517">
       <c r="A517" t="n">
@@ -10265,7 +10769,11 @@
           <t>http://ijes.info/index.html</t>
         </is>
       </c>
-      <c r="D517" t="inlineStr"/>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="518">
       <c r="A518" t="n">
@@ -10281,7 +10789,11 @@
           <t>http://www.jetir.org/</t>
         </is>
       </c>
-      <c r="D518" t="inlineStr"/>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="519">
       <c r="A519" t="n">
@@ -10297,7 +10809,11 @@
           <t>http://www.ijetr.org/</t>
         </is>
       </c>
-      <c r="D519" t="inlineStr"/>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="520">
       <c r="A520" t="n">
@@ -10313,7 +10829,11 @@
           <t>http://www.ijetae.com/index.html</t>
         </is>
       </c>
-      <c r="D520" t="inlineStr"/>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="521">
       <c r="A521" t="n">
@@ -10329,7 +10849,11 @@
           <t>http://www.ijetee.org/</t>
         </is>
       </c>
-      <c r="D521" t="inlineStr"/>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="522">
       <c r="A522" t="n">
@@ -10345,7 +10869,11 @@
           <t>http://ijetps.com/</t>
         </is>
       </c>
-      <c r="D522" t="inlineStr"/>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="523">
       <c r="A523" t="n">
@@ -10361,7 +10889,11 @@
           <t>http://www.ijoetr.com/</t>
         </is>
       </c>
-      <c r="D523" t="inlineStr"/>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="524">
       <c r="A524" t="n">
@@ -10377,7 +10909,11 @@
           <t>http://igmpublication.org/ijetst.in/</t>
         </is>
       </c>
-      <c r="D524" t="inlineStr"/>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="525">
       <c r="A525" t="n">
@@ -10393,7 +10929,11 @@
           <t>http://www.journal-enertech.eu/</t>
         </is>
       </c>
-      <c r="D525" t="inlineStr"/>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="526">
       <c r="A526" t="n">
@@ -10409,7 +10949,11 @@
           <t>http://international%20journal%20of%20energy%20and%20water%20resources%20%28ijewr%29/</t>
         </is>
       </c>
-      <c r="D526" t="inlineStr"/>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="527">
       <c r="A527" t="n">
@@ -10425,7 +10969,11 @@
           <t>http://www.ijesr.org/</t>
         </is>
       </c>
-      <c r="D527" t="inlineStr"/>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="528">
       <c r="A528" t="n">
@@ -10441,7 +10989,11 @@
           <t>https://www.ijeart.com/</t>
         </is>
       </c>
-      <c r="D528" t="inlineStr"/>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="529">
       <c r="A529" t="n">
@@ -10457,7 +11009,11 @@
           <t>http://www.ijeat.org/</t>
         </is>
       </c>
-      <c r="D529" t="inlineStr"/>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="530">
       <c r="A530" t="n">
@@ -10473,7 +11029,11 @@
           <t>http://eaas-journal.org/</t>
         </is>
       </c>
-      <c r="D530" t="inlineStr"/>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="531">
       <c r="A531" t="n">
@@ -10489,7 +11049,11 @@
           <t>http://www.ijeas.org/</t>
         </is>
       </c>
-      <c r="D531" t="inlineStr"/>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="532">
       <c r="A532" t="n">
@@ -10505,7 +11069,11 @@
           <t>http://www.ijecs.in/</t>
         </is>
       </c>
-      <c r="D532" t="inlineStr"/>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="533">
       <c r="A533" t="n">
@@ -10521,7 +11089,11 @@
           <t>http://ijeit.com/index.php</t>
         </is>
       </c>
-      <c r="D533" t="inlineStr"/>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="534">
       <c r="A534" t="n">
@@ -10537,7 +11109,11 @@
           <t>http://www.ijemr.net/</t>
         </is>
       </c>
-      <c r="D534" t="inlineStr"/>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="535">
       <c r="A535" t="n">
@@ -10553,7 +11129,11 @@
           <t>http://www.theijes.com/</t>
         </is>
       </c>
-      <c r="D535" t="inlineStr"/>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="536">
       <c r="A536" t="n">
@@ -10569,7 +11149,11 @@
           <t>http://www.ijesi.org/index.html</t>
         </is>
       </c>
-      <c r="D536" t="inlineStr"/>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="537">
       <c r="A537" t="n">
@@ -10585,7 +11169,11 @@
           <t>http://www.iet-journals.org/</t>
         </is>
       </c>
-      <c r="D537" t="inlineStr"/>
+      <c r="D537" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="538">
       <c r="A538" t="n">
@@ -10601,7 +11189,11 @@
           <t>http://www.ijetch.org/</t>
         </is>
       </c>
-      <c r="D538" t="inlineStr"/>
+      <c r="D538" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="539">
       <c r="A539" t="n">
@@ -10617,7 +11209,11 @@
           <t>http://www.ijeast.com/</t>
         </is>
       </c>
-      <c r="D539" t="inlineStr"/>
+      <c r="D539" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="540">
       <c r="A540" t="n">
@@ -10633,7 +11229,11 @@
           <t>http://ijea.jctjournals.com/</t>
         </is>
       </c>
-      <c r="D540" t="inlineStr"/>
+      <c r="D540" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="541">
       <c r="A541" t="n">
@@ -10649,7 +11249,11 @@
           <t>http://www.ijedr.org/index.php</t>
         </is>
       </c>
-      <c r="D541" t="inlineStr"/>
+      <c r="D541" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="542">
       <c r="A542" t="n">
@@ -10665,7 +11269,11 @@
           <t>http://ijeir.org/</t>
         </is>
       </c>
-      <c r="D542" t="inlineStr"/>
+      <c r="D542" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="543">
       <c r="A543" t="n">
@@ -10681,7 +11289,11 @@
           <t>http://www.ijeijournal.com/index.html</t>
         </is>
       </c>
-      <c r="D543" t="inlineStr"/>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="544">
       <c r="A544" t="n">
@@ -10697,7 +11309,11 @@
           <t>http://ijemcs.in/index.php/ijemcs</t>
         </is>
       </c>
-      <c r="D544" t="inlineStr"/>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="545">
       <c r="A545" t="n">
@@ -10713,7 +11329,11 @@
           <t>http://www.ijer.in/ijer/</t>
         </is>
       </c>
-      <c r="D545" t="inlineStr"/>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="546">
       <c r="A546" t="n">
@@ -10729,7 +11349,11 @@
           <t>http://www.ijera.com/index.html</t>
         </is>
       </c>
-      <c r="D546" t="inlineStr"/>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="547">
       <c r="A547" t="n">
@@ -10745,7 +11369,11 @@
           <t>http://ijercs.in/</t>
         </is>
       </c>
-      <c r="D547" t="inlineStr"/>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="548">
       <c r="A548" t="n">
@@ -10761,7 +11389,11 @@
           <t>http://www.ijerd.com/</t>
         </is>
       </c>
-      <c r="D548" t="inlineStr"/>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="549">
       <c r="A549" t="n">
@@ -10777,7 +11409,11 @@
           <t>http://www.ijergs.org/</t>
         </is>
       </c>
-      <c r="D549" t="inlineStr"/>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="550">
       <c r="A550" t="n">
@@ -10793,7 +11429,11 @@
           <t>https://www.ijerm.com/</t>
         </is>
       </c>
-      <c r="D550" t="inlineStr"/>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="551">
       <c r="A551" t="n">
@@ -10809,7 +11449,11 @@
           <t>http://www.ijoer.com/</t>
         </is>
       </c>
-      <c r="D551" t="inlineStr"/>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="552">
       <c r="A552" t="n">
@@ -10825,7 +11469,11 @@
           <t>http://www.ijerst.com/index.php</t>
         </is>
       </c>
-      <c r="D552" t="inlineStr"/>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="553">
       <c r="A553" t="n">
@@ -10841,7 +11489,11 @@
           <t>https://www.ijert.org/</t>
         </is>
       </c>
-      <c r="D553" t="inlineStr"/>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="554">
       <c r="A554" t="n">
@@ -10857,7 +11509,11 @@
           <t>http://www.ijerms.com/</t>
         </is>
       </c>
-      <c r="D554" t="inlineStr"/>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="555">
       <c r="A555" t="n">
@@ -10873,7 +11529,11 @@
           <t>http://ijesat.org/</t>
         </is>
       </c>
-      <c r="D555" t="inlineStr"/>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="556">
       <c r="A556" t="n">
@@ -10889,7 +11549,11 @@
           <t>http://ijesc.org/</t>
         </is>
       </c>
-      <c r="D556" t="inlineStr"/>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="557">
       <c r="A557" t="n">
@@ -10905,7 +11569,11 @@
           <t>http://ijesar.in/home/index</t>
         </is>
       </c>
-      <c r="D557" t="inlineStr"/>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="558">
       <c r="A558" t="n">
@@ -10921,7 +11589,11 @@
           <t>http://www.ijesit.com/</t>
         </is>
       </c>
-      <c r="D558" t="inlineStr"/>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="559">
       <c r="A559" t="n">
@@ -10937,7 +11609,11 @@
           <t>http://www.ijest-ng.com/</t>
         </is>
       </c>
-      <c r="D559" t="inlineStr"/>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="560">
       <c r="A560" t="n">
@@ -10953,7 +11629,11 @@
           <t>http://www.ijesird.com/</t>
         </is>
       </c>
-      <c r="D560" t="inlineStr"/>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="561">
       <c r="A561" t="n">
@@ -10969,7 +11649,11 @@
           <t>http://www.ijesrt.com/index.html</t>
         </is>
       </c>
-      <c r="D561" t="inlineStr"/>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="562">
       <c r="A562" t="n">
@@ -10985,7 +11669,11 @@
           <t>http://www.ijesmr.com/</t>
         </is>
       </c>
-      <c r="D562" t="inlineStr"/>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="563">
       <c r="A563" t="n">
@@ -11001,7 +11689,11 @@
           <t>http://www.ijetmr.com/index.html</t>
         </is>
       </c>
-      <c r="D563" t="inlineStr"/>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="564">
       <c r="A564" t="n">
@@ -11017,7 +11709,11 @@
           <t>http://ijetcr.org/</t>
         </is>
       </c>
-      <c r="D564" t="inlineStr"/>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="565">
       <c r="A565" t="n">
@@ -11033,7 +11729,11 @@
           <t>http://ijetm.org/</t>
         </is>
       </c>
-      <c r="D565" t="inlineStr"/>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="566">
       <c r="A566" t="n">
@@ -11049,7 +11749,11 @@
           <t>http://www.ijetsi.org/</t>
         </is>
       </c>
-      <c r="D566" t="inlineStr"/>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="567">
       <c r="A567" t="n">
@@ -11065,7 +11769,11 @@
           <t>http://www.ijetmas.com/</t>
         </is>
       </c>
-      <c r="D567" t="inlineStr"/>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="568">
       <c r="A568" t="n">
@@ -11081,7 +11789,11 @@
           <t>http://www.ijetajournal.org/</t>
         </is>
       </c>
-      <c r="D568" t="inlineStr"/>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="569">
       <c r="A569" t="n">
@@ -11097,7 +11809,11 @@
           <t>http://ijettjournal.org/</t>
         </is>
       </c>
-      <c r="D569" t="inlineStr"/>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="570">
       <c r="A570" t="n">
@@ -11113,7 +11829,11 @@
           <t>http://ijee.org/</t>
         </is>
       </c>
-      <c r="D570" t="inlineStr"/>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="571">
       <c r="A571" t="n">
@@ -11129,7 +11849,11 @@
           <t>http://eltsjournal.org/</t>
         </is>
       </c>
-      <c r="D571" t="inlineStr"/>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="572">
       <c r="A572" t="n">
@@ -11145,7 +11869,11 @@
           <t>http://ijellh.com/</t>
         </is>
       </c>
-      <c r="D572" t="inlineStr"/>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="573">
       <c r="A573" t="n">
@@ -11161,7 +11889,11 @@
           <t>http://www.ijelr.in/</t>
         </is>
       </c>
-      <c r="D573" t="inlineStr"/>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="574">
       <c r="A574" t="n">
@@ -11177,7 +11909,11 @@
           <t>http://www.englishresearchjournal.com/</t>
         </is>
       </c>
-      <c r="D574" t="inlineStr"/>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="575">
       <c r="A575" t="n">
@@ -11193,7 +11929,11 @@
           <t>http://www.ijecbs.com/</t>
         </is>
       </c>
-      <c r="D575" t="inlineStr"/>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="576">
       <c r="A576" t="n">
@@ -11209,7 +11949,11 @@
           <t>http://benjapan.org/ije/</t>
         </is>
       </c>
-      <c r="D576" t="inlineStr"/>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="577">
       <c r="A577" t="n">
@@ -11225,7 +11969,11 @@
           <t>http://www.ijoear.com/</t>
         </is>
       </c>
-      <c r="D577" t="inlineStr"/>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="578">
       <c r="A578" t="n">
@@ -11241,7 +11989,11 @@
           <t>http://ijeab.com/</t>
         </is>
       </c>
-      <c r="D578" t="inlineStr"/>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="579">
       <c r="A579" t="n">
@@ -11257,7 +12009,11 @@
           <t>http://www.ijesd.org/</t>
         </is>
       </c>
-      <c r="D579" t="inlineStr"/>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="580">
       <c r="A580" t="n">
@@ -11273,7 +12029,11 @@
           <t>http://ijfas.com/</t>
         </is>
       </c>
-      <c r="D580" t="inlineStr"/>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="581">
       <c r="A581" t="n">
@@ -11289,7 +12049,11 @@
           <t>http://www.faunajournal.com/</t>
         </is>
       </c>
-      <c r="D581" t="inlineStr"/>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="582">
       <c r="A582" t="n">
@@ -11305,7 +12069,11 @@
           <t>http://www.fisheriesjournal.com/</t>
         </is>
       </c>
-      <c r="D582" t="inlineStr"/>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="583">
       <c r="A583" t="n">
@@ -11321,7 +12089,11 @@
           <t>http://www.ijfans.com/index.php</t>
         </is>
       </c>
-      <c r="D583" t="inlineStr"/>
+      <c r="D583" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="584">
       <c r="A584" t="n">
@@ -11337,7 +12109,11 @@
           <t>http://www.bma.org.in/IJFAS.aspx</t>
         </is>
       </c>
-      <c r="D584" t="inlineStr"/>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="585">
       <c r="A585" t="n">
@@ -11353,7 +12129,11 @@
           <t>http://ijgc.jalaxy.com.tw/</t>
         </is>
       </c>
-      <c r="D585" t="inlineStr"/>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="586">
       <c r="A586" t="n">
@@ -11369,7 +12149,11 @@
           <t>http://journalglobalideas.com/</t>
         </is>
       </c>
-      <c r="D586" t="inlineStr"/>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="587">
       <c r="A587" t="n">
@@ -11385,7 +12169,11 @@
           <t>http://www.ijgovernance.com/</t>
         </is>
       </c>
-      <c r="D587" t="inlineStr"/>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="588">
       <c r="A588" t="n">
@@ -11401,7 +12189,11 @@
           <t>http://www.ijghc.com/</t>
         </is>
       </c>
-      <c r="D588" t="inlineStr"/>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="589">
       <c r="A589" t="n">
@@ -11417,7 +12209,11 @@
           <t>http://www.ijhr.org/</t>
         </is>
       </c>
-      <c r="D589" t="inlineStr"/>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="590">
       <c r="A590" t="n">
@@ -11433,7 +12229,11 @@
           <t>http://ijhrmims.com/index.php</t>
         </is>
       </c>
-      <c r="D590" t="inlineStr"/>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="591">
       <c r="A591" t="n">
@@ -11449,7 +12249,11 @@
           <t>http://www.ijhsr.org/</t>
         </is>
       </c>
-      <c r="D591" t="inlineStr"/>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="592">
       <c r="A592" t="n">
@@ -11465,7 +12269,11 @@
           <t>http://www.florajournal.com/</t>
         </is>
       </c>
-      <c r="D592" t="inlineStr"/>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="593">
       <c r="A593" t="n">
@@ -11481,7 +12289,11 @@
           <t>http://www.hindijournal.com/</t>
         </is>
       </c>
-      <c r="D593" t="inlineStr"/>
+      <c r="D593" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="594">
       <c r="A594" t="n">
@@ -11497,7 +12309,11 @@
           <t>http://newhistoryjournal.com/</t>
         </is>
       </c>
-      <c r="D594" t="inlineStr"/>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="595">
       <c r="A595" t="n">
@@ -11513,7 +12329,11 @@
           <t>http://www.homesciencejournal.com/board.html</t>
         </is>
       </c>
-      <c r="D595" t="inlineStr"/>
+      <c r="D595" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="596">
       <c r="A596" t="n">
@@ -11529,7 +12349,11 @@
           <t>http://www.ijsse.org/index.php?option=com_content&amp;view=article&amp;id=69&amp;Itemid=68</t>
         </is>
       </c>
-      <c r="D596" t="inlineStr"/>
+      <c r="D596" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="597">
       <c r="A597" t="n">
@@ -11545,7 +12369,11 @@
           <t>http://www.j-humansciences.com/</t>
         </is>
       </c>
-      <c r="D597" t="inlineStr"/>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="598">
       <c r="A598" t="n">
@@ -11561,7 +12389,11 @@
           <t>http://www.ijhcs.com/index.php/ijhcs</t>
         </is>
       </c>
-      <c r="D598" t="inlineStr"/>
+      <c r="D598" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="599">
       <c r="A599" t="n">
@@ -11577,7 +12409,11 @@
           <t>http://www.ijhssi.org/</t>
         </is>
       </c>
-      <c r="D599" t="inlineStr"/>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="600">
       <c r="A600" t="n">
@@ -11593,7 +12429,11 @@
           <t>http://www.socialresearchjournals.com/</t>
         </is>
       </c>
-      <c r="D600" t="inlineStr"/>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="601">
       <c r="A601" t="n">
@@ -11609,7 +12449,11 @@
           <t>http://www.theijhss.com/</t>
         </is>
       </c>
-      <c r="D601" t="inlineStr"/>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="602">
       <c r="A602" t="n">
@@ -11625,7 +12469,11 @@
           <t>http://aajhss.org/index.php/ijhss/index</t>
         </is>
       </c>
-      <c r="D602" t="inlineStr"/>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="603">
       <c r="A603" t="n">
@@ -11641,7 +12489,11 @@
           <t>http://humanitiesjournal.info/index.php/ijhr/</t>
         </is>
       </c>
-      <c r="D603" t="inlineStr"/>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="604">
       <c r="A604" t="n">
@@ -11657,7 +12509,11 @@
           <t>http://ijheps.org/</t>
         </is>
       </c>
-      <c r="D604" t="inlineStr"/>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="605">
       <c r="A605" t="n">
@@ -11673,7 +12529,11 @@
           <t>http://ijip.in/</t>
         </is>
       </c>
-      <c r="D605" t="inlineStr"/>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="606">
       <c r="A606" t="n">
@@ -11689,7 +12549,11 @@
           <t>http://esjournals.org/index.php</t>
         </is>
       </c>
-      <c r="D606" t="inlineStr"/>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="607">
       <c r="A607" t="n">
@@ -11705,7 +12569,11 @@
           <t>http://www.ijictt.ictt.info/</t>
         </is>
       </c>
-      <c r="D607" t="inlineStr"/>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="608">
       <c r="A608" t="n">
@@ -11721,7 +12589,11 @@
           <t>http://www.ijiet.org/</t>
         </is>
       </c>
-      <c r="D608" t="inlineStr"/>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="609">
       <c r="A609" t="n">
@@ -11737,7 +12609,11 @@
           <t>http://www.spoars.org/journal/</t>
         </is>
       </c>
-      <c r="D609" t="inlineStr"/>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="610">
       <c r="A610" t="n">
@@ -11753,7 +12629,11 @@
           <t>http://www.ijirr.com/</t>
         </is>
       </c>
-      <c r="D610" t="inlineStr"/>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="611">
       <c r="A611" t="n">
@@ -11769,7 +12649,11 @@
           <t>http://www.ijss.in/</t>
         </is>
       </c>
-      <c r="D611" t="inlineStr"/>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="612">
       <c r="A612" t="n">
@@ -11785,7 +12669,11 @@
           <t>http://www.jitbm.com/</t>
         </is>
       </c>
-      <c r="D612" t="inlineStr"/>
+      <c r="D612" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="613">
       <c r="A613" t="n">
@@ -11801,7 +12689,11 @@
           <t>http://ijitcs.com/</t>
         </is>
       </c>
-      <c r="D613" t="inlineStr"/>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="614">
       <c r="A614" t="n">
@@ -11817,7 +12709,11 @@
           <t>http://www.iteejournal.org/</t>
         </is>
       </c>
-      <c r="D614" t="inlineStr"/>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="615">
       <c r="A615" t="n">
@@ -11833,7 +12729,11 @@
           <t>http://ijifr.com/</t>
         </is>
       </c>
-      <c r="D615" t="inlineStr"/>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="616">
       <c r="A616" t="n">
@@ -11849,7 +12749,11 @@
           <t>http://www.ijires.org/</t>
         </is>
       </c>
-      <c r="D616" t="inlineStr"/>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="617">
       <c r="A617" t="n">
@@ -11865,7 +12769,11 @@
           <t>http://www.ijism.org/</t>
         </is>
       </c>
-      <c r="D617" t="inlineStr"/>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="618">
       <c r="A618" t="n">
@@ -11881,7 +12789,11 @@
           <t>http://www.journalijir.com/</t>
         </is>
       </c>
-      <c r="D618" t="inlineStr"/>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="619">
       <c r="A619" t="n">
@@ -11897,7 +12809,11 @@
           <t>http://ijiet.com/</t>
         </is>
       </c>
-      <c r="D619" t="inlineStr"/>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="620">
       <c r="A620" t="n">
@@ -11913,7 +12829,11 @@
           <t>http://www.ijiert.org/</t>
         </is>
       </c>
-      <c r="D620" t="inlineStr"/>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="621">
       <c r="A621" t="n">
@@ -11929,7 +12849,11 @@
           <t>http://www.ijisr.com/</t>
         </is>
       </c>
-      <c r="D621" t="inlineStr"/>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="622">
       <c r="A622" t="n">
@@ -11945,7 +12869,11 @@
           <t>http://journalijiar.com/</t>
         </is>
       </c>
-      <c r="D622" t="inlineStr"/>
+      <c r="D622" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="623">
       <c r="A623" t="n">
@@ -11961,7 +12889,11 @@
           <t>http://ijiere.com/</t>
         </is>
       </c>
-      <c r="D623" t="inlineStr"/>
+      <c r="D623" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="624">
       <c r="A624" t="n">
@@ -11977,7 +12909,11 @@
           <t>http://ijicse.in/</t>
         </is>
       </c>
-      <c r="D624" t="inlineStr"/>
+      <c r="D624" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="625">
       <c r="A625" t="n">
@@ -11993,7 +12929,11 @@
           <t>http://www.ijicr.com/</t>
         </is>
       </c>
-      <c r="D625" t="inlineStr"/>
+      <c r="D625" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="626">
       <c r="A626" t="n">
@@ -12009,7 +12949,11 @@
           <t>http://www.publishtopublic.com/</t>
         </is>
       </c>
-      <c r="D626" t="inlineStr"/>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="627">
       <c r="A627" t="n">
@@ -12025,7 +12969,11 @@
           <t>http://www.auamii.com/journal.html</t>
         </is>
       </c>
-      <c r="D627" t="inlineStr"/>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="628">
       <c r="A628" t="n">
@@ -12041,7 +12989,11 @@
           <t>http://www.ijipr.com/</t>
         </is>
       </c>
-      <c r="D628" t="inlineStr"/>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="629">
       <c r="A629" t="n">
@@ -12057,7 +13009,11 @@
           <t>http://www.ijiras.com/</t>
         </is>
       </c>
-      <c r="D629" t="inlineStr"/>
+      <c r="D629" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="630">
       <c r="A630" t="n">
@@ -12073,7 +13029,11 @@
           <t>http://www.ijirct.org/index.php</t>
         </is>
       </c>
-      <c r="D630" t="inlineStr"/>
+      <c r="D630" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="631">
       <c r="A631" t="n">
@@ -12089,7 +13049,11 @@
           <t>http://www.ijird.com/</t>
         </is>
       </c>
-      <c r="D631" t="inlineStr"/>
+      <c r="D631" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="632">
       <c r="A632" t="n">
@@ -12105,7 +13069,11 @@
           <t>http://www.ijirs.com/</t>
         </is>
       </c>
-      <c r="D632" t="inlineStr"/>
+      <c r="D632" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="633">
       <c r="A633" t="n">
@@ -12121,7 +13089,11 @@
           <t>http://ijirae.com/</t>
         </is>
       </c>
-      <c r="D633" t="inlineStr"/>
+      <c r="D633" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="634">
       <c r="A634" t="n">
@@ -12137,7 +13109,11 @@
           <t>http://www.ijircce.com/</t>
         </is>
       </c>
-      <c r="D634" t="inlineStr"/>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="635">
       <c r="A635" t="n">
@@ -12153,7 +13129,11 @@
           <t>http://www.ijireeice.com/</t>
         </is>
       </c>
-      <c r="D635" t="inlineStr"/>
+      <c r="D635" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="636">
       <c r="A636" t="n">
@@ -12169,7 +13149,11 @@
           <t>http://www.ijircst.org/</t>
         </is>
       </c>
-      <c r="D636" t="inlineStr"/>
+      <c r="D636" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="637">
       <c r="A637" t="n">
@@ -12185,7 +13169,11 @@
           <t>http://ijirmps.com/</t>
         </is>
       </c>
-      <c r="D637" t="inlineStr"/>
+      <c r="D637" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="638">
       <c r="A638" t="n">
@@ -12201,7 +13189,11 @@
           <t>http://www.ijirem.org/IJIREM/Home.aspx</t>
         </is>
       </c>
-      <c r="D638" t="inlineStr"/>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="639">
       <c r="A639" t="n">
@@ -12217,7 +13209,11 @@
           <t>http://ijirms.in/</t>
         </is>
       </c>
-      <c r="D639" t="inlineStr"/>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="640">
       <c r="A640" t="n">
@@ -12233,7 +13229,11 @@
           <t>http://www.ijirse.in/index.html</t>
         </is>
       </c>
-      <c r="D640" t="inlineStr"/>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="641">
       <c r="A641" t="n">
@@ -12249,7 +13249,11 @@
           <t>http://www.ijirset.com/</t>
         </is>
       </c>
-      <c r="D641" t="inlineStr"/>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="642">
       <c r="A642" t="n">
@@ -12265,7 +13269,11 @@
           <t>http://www.ijirt.org/index.php</t>
         </is>
       </c>
-      <c r="D642" t="inlineStr"/>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="643">
       <c r="A643" t="n">
@@ -12281,7 +13289,11 @@
           <t>http://www.ijirts.org/</t>
         </is>
       </c>
-      <c r="D643" t="inlineStr"/>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="644">
       <c r="A644" t="n">
@@ -12297,7 +13309,11 @@
           <t>http://www.ijiset.com/</t>
         </is>
       </c>
-      <c r="D644" t="inlineStr"/>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="645">
       <c r="A645" t="n">
@@ -12313,7 +13329,11 @@
           <t>http://www.ijisme.org/</t>
         </is>
       </c>
-      <c r="D645" t="inlineStr"/>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="646">
       <c r="A646" t="n">
@@ -12329,7 +13349,11 @@
           <t>http://ijisset.org/</t>
         </is>
       </c>
-      <c r="D646" t="inlineStr"/>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="647">
       <c r="A647" t="n">
@@ -12345,7 +13369,11 @@
           <t>http://ijitech.org/index.php</t>
         </is>
       </c>
-      <c r="D647" t="inlineStr"/>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="648">
       <c r="A648" t="n">
@@ -12361,7 +13389,11 @@
           <t>http://www.ijitee.org/</t>
         </is>
       </c>
-      <c r="D648" t="inlineStr"/>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="649">
       <c r="A649" t="n">
@@ -12377,7 +13409,11 @@
           <t>http://www.ijitr.com/</t>
         </is>
       </c>
-      <c r="D649" t="inlineStr"/>
+      <c r="D649" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="650">
       <c r="A650" t="n">
@@ -12393,7 +13429,11 @@
           <t>http://www.ijite.com/</t>
         </is>
       </c>
-      <c r="D650" t="inlineStr"/>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="651">
       <c r="A651" t="n">
@@ -12409,7 +13449,11 @@
           <t>http://ijicar.net/</t>
         </is>
       </c>
-      <c r="D651" t="inlineStr"/>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="652">
       <c r="A652" t="n">
@@ -12425,7 +13469,11 @@
           <t>http://www.ijoimr.com/</t>
         </is>
       </c>
-      <c r="D652" t="inlineStr"/>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="653">
       <c r="A653" t="n">
@@ -12441,7 +13489,11 @@
           <t>http://www.ijims.com/current.php</t>
         </is>
       </c>
-      <c r="D653" t="inlineStr"/>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="654">
       <c r="A654" t="n">
@@ -12457,7 +13509,11 @@
           <t>http://ijirssc.in/site/</t>
         </is>
       </c>
-      <c r="D654" t="inlineStr"/>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="655">
       <c r="A655" t="n">
@@ -12473,7 +13529,11 @@
           <t>http://www.ijips.net/</t>
         </is>
       </c>
-      <c r="D655" t="inlineStr"/>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="656">
       <c r="A656" t="n">
@@ -12489,7 +13549,11 @@
           <t>http://www.ijies.org/</t>
         </is>
       </c>
-      <c r="D656" t="inlineStr"/>
+      <c r="D656" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="657">
       <c r="A657" t="n">
@@ -12505,7 +13569,11 @@
           <t>http://ijkie.org/index.html</t>
         </is>
       </c>
-      <c r="D657" t="inlineStr"/>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="658">
       <c r="A658" t="n">
@@ -12521,7 +13589,11 @@
           <t>http://www.khatesefid.com/journal/index.html</t>
         </is>
       </c>
-      <c r="D658" t="inlineStr"/>
+      <c r="D658" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="659">
       <c r="A659" t="n">
@@ -12537,7 +13609,11 @@
           <t>http://www.ijllalw.org/</t>
         </is>
       </c>
-      <c r="D659" t="inlineStr"/>
+      <c r="D659" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="660">
       <c r="A660" t="n">
@@ -24249,7 +25325,11 @@
           <t>https://www.ijcsmc.com/</t>
         </is>
       </c>
-      <c r="D1391" t="inlineStr"/>
+      <c r="D1391" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="1392">
       <c r="A1392" t="n">
@@ -36509,7 +37589,11 @@
           <t>http://journalijcms.com/</t>
         </is>
       </c>
-      <c r="D2156" t="inlineStr"/>
+      <c r="D2156" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
     <row r="2157">
       <c r="A2157" t="n">

</xml_diff>